<commit_message>
Adding classes+Starting UserManager + add doc
</commit_message>
<xml_diff>
--- a/EvenementsEnDirect/docs/analyse/Journal de bord TPI DAvila 2020.xlsx
+++ b/EvenementsEnDirect/docs/analyse/Journal de bord TPI DAvila 2020.xlsx
@@ -18,6 +18,116 @@
   </si>
   <si>
     <t xml:space="preserve">INFORMATIONS GENERALES
+Date : 26/05/2020
+Elèves : Davila Lou
+</t>
+  </si>
+  <si>
+    <r>
+      <t>ÉTAPE DU PROJET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> : Analyse/Implémentation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BILAN : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>La phase d'analyse est terminée et l'implémentation commencée</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">
+Réalisé :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Création du MCD, création des utilisateurs de la base, mise en place de la structure du projet,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
+      <t>documentation d'analyse + doc technique,Implémentation BDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">
+A réaliser :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> Documentation technique,réalisation des Manager</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Éventuelle(s) DIFFICULTÉ(S) :  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">Pas de difficulté  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SOLUTIONS PROPOSÉES :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> Pas de difficulté donc pas de solution</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PROCHAINE ÉTAPE DU PROJET : </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>Implémentation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Observations particulières : </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>rdv journalier de 16 à 17h45 avec monsieur Aigroz. J'ai également ajouter de nouvelles maquettes et modifié certaines d'entre elles.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">INFORMATIONS GENERALES
 Date : 25/05/2020
 Elèves : Davila Lou
 </t>
@@ -111,105 +221,7 @@
     </r>
     <r>
       <rPr/>
-      <t>J'ai du refaire mes maquettes après avoir constaté qu'elles contenaient du français ET de l'anglais, j'ai donc uniformisé le tout ce qui m'a pris un peu plus de temps que prévu</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">INFORMATIONS GENERALES
-Date : 26/05/2020
-Elèves : Davila Lou
-</t>
-  </si>
-  <si>
-    <r>
-      <t>ÉTAPE DU PROJET</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve"> : Analyse/Implémentation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">BILAN : </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>La phase d'analyse est terminée et l'implémentation commencée</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">
-Réalisé :
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.0"/>
-      </rPr>
-      <t>Lecture de l'énoncé, Planification, Maquettage des vues, Une partie de la doc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">
-A réaliser :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve"> Documentation d'analyse, MCD, création des utilisateurs de la base, Mise en place de la structure du projet</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Éventuelle(s) DIFFICULTÉ(S) :  </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">Pas de difficulté  </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>SOLUTIONS PROPOSÉES :</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve"> Pas de difficulté donc pas de solution</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">PROCHAINE ÉTAPE DU PROJET : </t>
-    </r>
-    <r>
-      <rPr/>
-      <t>Finition de l'analyse/Implémentation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Observations particulières : </t>
-    </r>
-    <r>
-      <rPr/>
-      <t>J'ai du refaire mes maquettes après avoir constaté qu'elles contenaient du français ET de l'anglais, j'ai donc uniformisé le tout ce qui m'a pris un peu plus de temps que prévu</t>
+      <t>J'ai du refaire mes maquettes après avoir constaté qu'elles contenaient du français ET de l'anglais, j'ai donc uniformisé le tout ce qui m'a pris un peu plus de temps que prévu. J'ai également assisté au rdv journalier à 16h avec Monsieur Aigroz afin de faire le point sur cette première journée.</t>
     </r>
   </si>
 </sst>
@@ -234,14 +246,14 @@
     </font>
     <font>
       <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font/>
-    <font>
-      <b/>
-      <name val="Arial"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -346,17 +358,17 @@
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -639,8 +651,8 @@
       <c r="Z2" s="5"/>
     </row>
     <row r="3" ht="132.0" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
+      <c r="A3" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="5"/>
@@ -670,7 +682,7 @@
     </row>
     <row r="4" ht="143.25" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="5"/>
@@ -699,10 +711,10 @@
       <c r="Z4" s="5"/>
     </row>
     <row r="5" ht="129.0" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="10"/>
+      <c r="A5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="11"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -729,10 +741,10 @@
       <c r="Z5" s="5"/>
     </row>
     <row r="6" ht="107.25" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10"/>
+      <c r="A6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="11"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -759,10 +771,10 @@
       <c r="Z6" s="5"/>
     </row>
     <row r="7" ht="108.0" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="10"/>
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="11"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -789,10 +801,10 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8" ht="114.75" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="10"/>
+      <c r="A8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -819,10 +831,10 @@
       <c r="Z8" s="5"/>
     </row>
     <row r="9" ht="164.25" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="10"/>
+      <c r="A9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="11"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -934,8 +946,8 @@
       <c r="Z2" s="5"/>
     </row>
     <row r="3" ht="132.0" customHeight="1">
-      <c r="A3" s="11" t="s">
-        <v>8</v>
+      <c r="A3" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="5"/>
@@ -965,7 +977,7 @@
     </row>
     <row r="4" ht="143.25" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="5"/>
@@ -994,10 +1006,10 @@
       <c r="Z4" s="5"/>
     </row>
     <row r="5" ht="129.0" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="10"/>
+      <c r="A5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1024,10 +1036,10 @@
       <c r="Z5" s="5"/>
     </row>
     <row r="6" ht="107.25" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="10"/>
+      <c r="A6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1054,10 +1066,10 @@
       <c r="Z6" s="5"/>
     </row>
     <row r="7" ht="108.0" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="10"/>
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -1084,10 +1096,10 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8" ht="114.75" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="10"/>
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -1114,10 +1126,10 @@
       <c r="Z8" s="5"/>
     </row>
     <row r="9" ht="164.25" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="10"/>
+      <c r="A9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>

</xml_diff>